<commit_message>
edit plan make document
</commit_message>
<xml_diff>
--- a/Lending/20181205 - uiux.api.investigation.cmc.plan.draft.xlsx
+++ b/Lending/20181205 - uiux.api.investigation.cmc.plan.draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHOAND\DOCUMENT\OCB_DRIVER\VPB OCB\90 Work Orders\Work Order 0004\UIUX Project\Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces_2018\DemoSAP_UI5_Git\SAPUI_DEMO\Lending\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D72FBA7-3602-4887-9238-56E8C00C0979}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A1FDFE-F336-4D8D-8902-760D80B14229}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D4-6" sheetId="1" r:id="rId1"/>
@@ -1049,7 +1049,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1811,10 +1838,10 @@
   <dimension ref="A1:S186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1917,7 @@
       </c>
       <c r="Q1" s="4" t="str">
         <f>"Open: " &amp; COUNTIF($K$2:$K$70,"Open")</f>
-        <v>Open: 31</v>
+        <v>Open: 30</v>
       </c>
       <c r="R1" s="4" t="str">
         <f>"WIP: " &amp; COUNTIF($K$2:$K$70,"WIP")</f>
@@ -1898,7 +1925,7 @@
       </c>
       <c r="S1" s="4" t="str">
         <f>"Done: " &amp; COUNTIF($K$2:$K$70,"Done")</f>
-        <v>Done: 18</v>
+        <v>Done: 19</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="11" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2779,7 +2806,7 @@
         <v>252</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L24" s="19"/>
       <c r="M24" s="24"/>
@@ -2896,7 +2923,7 @@
         <v>70</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="L27" s="19"/>
       <c r="M27" s="21"/>
@@ -2933,11 +2960,11 @@
       <c r="I28" s="35">
         <v>43462</v>
       </c>
-      <c r="J28" s="36" t="s">
-        <v>106</v>
+      <c r="J28" s="23" t="s">
+        <v>252</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="21"/>
@@ -2976,7 +3003,7 @@
         <v>70</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="L29" s="19"/>
       <c r="M29" s="21"/>
@@ -4753,11 +4780,16 @@
         <filter val="UPL"/>
       </filters>
     </filterColumn>
-    <sortState ref="A9:N39">
-      <sortCondition ref="H1:H186"/>
-    </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="K187:L1048576 K66:L183 N64:N70 N53 K25:L63 K1:L22">
+  <conditionalFormatting sqref="K187:L1048576 K66:L183 N64:N70 N53 K1:L22 K25:L63">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"WIP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
@@ -4765,7 +4797,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1">
+  <conditionalFormatting sqref="M1">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
@@ -4773,7 +4805,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1">
+  <conditionalFormatting sqref="K184:L186">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
@@ -4781,7 +4813,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K184:L186">
+  <conditionalFormatting sqref="K64:L65">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
@@ -4789,7 +4821,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K64:L65">
+  <conditionalFormatting sqref="K24">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add Feature - List Services UIUX 04.01.2019 -Plan mapping code OCB.xlsx
</commit_message>
<xml_diff>
--- a/Lending/20181205 - uiux.api.investigation.cmc.plan.draft.xlsx
+++ b/Lending/20181205 - uiux.api.investigation.cmc.plan.draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces_2018\DemoSAP_UI5_Git\SAPUI_DEMO\Lending\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B00927-A33A-4135-BE7B-C3228D113477}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD6FEE9-20E6-4355-BF29-7C4BDC853B7D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Desktop:</t>
         </r>
@@ -57,7 +57,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 trùng với Loan Detail
@@ -878,7 +878,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-101042A]d\ mmm\ yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -925,17 +925,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1877,10 +1871,10 @@
   <dimension ref="A1:S186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="G192" sqref="G192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.25"/>
@@ -2226,7 +2220,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
         <v>110</v>
@@ -2263,7 +2257,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
@@ -2302,7 +2296,7 @@
       <c r="N10" s="24"/>
       <c r="O10" s="19"/>
     </row>
-    <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>31</v>
       </c>
@@ -2382,7 +2376,7 @@
       </c>
       <c r="O12" s="19"/>
     </row>
-    <row r="13" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>31</v>
       </c>
@@ -2421,7 +2415,7 @@
       <c r="N13" s="24"/>
       <c r="O13" s="19"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>31</v>
       </c>
@@ -2460,7 +2454,7 @@
       <c r="N14" s="24"/>
       <c r="O14" s="19"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
         <v>138</v>
@@ -2497,7 +2491,7 @@
       <c r="N15" s="24"/>
       <c r="O15" s="19"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>31</v>
       </c>
@@ -2536,7 +2530,7 @@
       <c r="N16" s="24"/>
       <c r="O16" s="19"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>31</v>
       </c>
@@ -2575,7 +2569,7 @@
       <c r="N17" s="24"/>
       <c r="O17" s="19"/>
     </row>
-    <row r="18" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>31</v>
       </c>
@@ -2614,7 +2608,7 @@
       <c r="N18" s="24"/>
       <c r="O18" s="19"/>
     </row>
-    <row r="19" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>31</v>
       </c>
@@ -2655,7 +2649,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>31</v>
       </c>
@@ -2696,7 +2690,7 @@
       </c>
       <c r="O20" s="19"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>31</v>
       </c>
@@ -2735,7 +2729,7 @@
       <c r="N21" s="24"/>
       <c r="O21" s="19"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>31</v>
       </c>
@@ -2774,7 +2768,7 @@
       <c r="N22" s="24"/>
       <c r="O22" s="19"/>
     </row>
-    <row r="23" spans="1:15" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="16" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>14</v>
       </c>
@@ -3172,7 +3166,7 @@
       <c r="N32" s="24"/>
       <c r="O32" s="19"/>
     </row>
-    <row r="33" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>31</v>
       </c>
@@ -3211,7 +3205,7 @@
       <c r="N33" s="24"/>
       <c r="O33" s="19"/>
     </row>
-    <row r="34" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>31</v>
       </c>
@@ -3250,7 +3244,7 @@
       <c r="N34" s="24"/>
       <c r="O34" s="19"/>
     </row>
-    <row r="35" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>31</v>
       </c>
@@ -3289,7 +3283,7 @@
       <c r="N35" s="24"/>
       <c r="O35" s="19"/>
     </row>
-    <row r="36" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>31</v>
       </c>
@@ -3320,7 +3314,7 @@
       <c r="N36" s="24"/>
       <c r="O36" s="19"/>
     </row>
-    <row r="37" spans="1:15" s="16" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="16" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19" t="s">
@@ -3341,7 +3335,7 @@
       <c r="N37" s="24"/>
       <c r="O37" s="19"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19" t="s">
@@ -3362,7 +3356,7 @@
       <c r="N38" s="24"/>
       <c r="O38" s="19"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="19" t="s">
         <v>141</v>
@@ -4813,10 +4807,7 @@
   <autoFilter ref="A1:N186" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Loan"/>
-        <filter val="Overdraft"/>
         <filter val="Saving"/>
-        <filter val="UPL"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>